<commit_message>
Quiz07 and 08 and Grades and Homework03-Tutorial03
</commit_message>
<xml_diff>
--- a/phy112/Grades/grades_report_2023.xlsx
+++ b/phy112/Grades/grades_report_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ptohos/Documents/MyCourses/FYS112/2023/Grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AAA75B-522A-244B-8054-797E85BF9464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F989E3-9B67-CF42-B4BC-675ACF0803B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="500" windowWidth="32900" windowHeight="19240" tabRatio="334" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="500" windowWidth="32900" windowHeight="19240" tabRatio="334" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quiz" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -995,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -1081,26 +1081,30 @@
       <c r="A2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="59">
-        <v>3</v>
-      </c>
-      <c r="C2" s="59">
-        <v>15</v>
-      </c>
-      <c r="D2" s="59">
+      <c r="B2" s="55">
+        <v>3</v>
+      </c>
+      <c r="C2" s="55">
+        <v>15</v>
+      </c>
+      <c r="D2" s="55">
         <v>12</v>
       </c>
-      <c r="E2" s="59">
-        <v>3</v>
-      </c>
-      <c r="F2" s="18">
-        <v>3</v>
-      </c>
-      <c r="G2" s="18">
-        <v>3</v>
-      </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="E2" s="55">
+        <v>3</v>
+      </c>
+      <c r="F2" s="49">
+        <v>3</v>
+      </c>
+      <c r="G2" s="49">
+        <v>3</v>
+      </c>
+      <c r="H2" s="49">
+        <v>3</v>
+      </c>
+      <c r="I2" s="18">
+        <v>3</v>
+      </c>
       <c r="J2" s="49"/>
       <c r="K2" s="49"/>
       <c r="L2" s="49"/>
@@ -1115,7 +1119,7 @@
       <c r="U2" s="49"/>
       <c r="V2" s="39">
         <f>$V$35 * ( (SUM(B2:U2))/((SUM($B$39:$U$39))*$B$35) )</f>
-        <v>0.43333333333333335</v>
+        <v>0.375</v>
       </c>
       <c r="W2"/>
     </row>
@@ -1123,26 +1127,30 @@
       <c r="A3" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="59">
-        <v>15</v>
-      </c>
-      <c r="C3" s="59">
-        <v>15</v>
-      </c>
-      <c r="D3" s="59">
+      <c r="B3" s="55">
+        <v>15</v>
+      </c>
+      <c r="C3" s="55">
+        <v>15</v>
+      </c>
+      <c r="D3" s="55">
         <v>12</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="55">
         <v>8</v>
       </c>
-      <c r="F3" s="18">
-        <v>15</v>
-      </c>
-      <c r="G3" s="18">
-        <v>3</v>
-      </c>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
+      <c r="F3" s="49">
+        <v>15</v>
+      </c>
+      <c r="G3" s="49">
+        <v>3</v>
+      </c>
+      <c r="H3" s="49">
+        <v>8</v>
+      </c>
+      <c r="I3" s="18">
+        <v>3</v>
+      </c>
       <c r="J3" s="49"/>
       <c r="K3" s="49"/>
       <c r="L3" s="49"/>
@@ -1157,7 +1165,7 @@
       <c r="U3" s="49"/>
       <c r="V3" s="39">
         <f t="shared" ref="V3:V33" si="0">$V$35 * ( (SUM(B3:U3))/((SUM($B$39:$U$39))*$B$35) )</f>
-        <v>0.75555555555555554</v>
+        <v>0.65833333333333333</v>
       </c>
       <c r="W3"/>
     </row>
@@ -1165,26 +1173,30 @@
       <c r="A4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="59">
-        <v>0</v>
-      </c>
-      <c r="C4" s="59">
-        <v>0</v>
-      </c>
-      <c r="D4" s="59">
-        <v>0</v>
-      </c>
-      <c r="E4" s="59">
-        <v>0</v>
-      </c>
-      <c r="F4" s="18">
-        <v>0</v>
-      </c>
-      <c r="G4" s="18">
-        <v>0</v>
-      </c>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
+      <c r="B4" s="55">
+        <v>0</v>
+      </c>
+      <c r="C4" s="55">
+        <v>0</v>
+      </c>
+      <c r="D4" s="55">
+        <v>0</v>
+      </c>
+      <c r="E4" s="55">
+        <v>0</v>
+      </c>
+      <c r="F4" s="49">
+        <v>0</v>
+      </c>
+      <c r="G4" s="49">
+        <v>0</v>
+      </c>
+      <c r="H4" s="49">
+        <v>0</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0</v>
+      </c>
       <c r="J4" s="49"/>
       <c r="K4" s="49"/>
       <c r="L4" s="49"/>
@@ -1207,26 +1219,30 @@
       <c r="A5" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="59">
-        <v>3</v>
-      </c>
-      <c r="C5" s="59">
-        <v>15</v>
-      </c>
-      <c r="D5" s="59">
+      <c r="B5" s="55">
+        <v>3</v>
+      </c>
+      <c r="C5" s="55">
+        <v>15</v>
+      </c>
+      <c r="D5" s="55">
         <v>12</v>
       </c>
-      <c r="E5" s="59">
-        <v>15</v>
-      </c>
-      <c r="F5" s="18">
-        <v>0</v>
-      </c>
-      <c r="G5" s="18">
-        <v>3</v>
-      </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="E5" s="55">
+        <v>15</v>
+      </c>
+      <c r="F5" s="49">
+        <v>0</v>
+      </c>
+      <c r="G5" s="49">
+        <v>3</v>
+      </c>
+      <c r="H5" s="49">
+        <v>3</v>
+      </c>
+      <c r="I5" s="18">
+        <v>3</v>
+      </c>
       <c r="J5" s="49"/>
       <c r="K5" s="49"/>
       <c r="L5" s="49"/>
@@ -1241,7 +1257,7 @@
       <c r="U5" s="49"/>
       <c r="V5" s="39">
         <f t="shared" si="0"/>
-        <v>0.53333333333333333</v>
+        <v>0.45</v>
       </c>
       <c r="W5"/>
     </row>
@@ -1249,26 +1265,30 @@
       <c r="A6" s="29">
         <v>1019</v>
       </c>
-      <c r="B6" s="59">
-        <v>15</v>
-      </c>
-      <c r="C6" s="59">
-        <v>15</v>
-      </c>
-      <c r="D6" s="59">
-        <v>15</v>
-      </c>
-      <c r="E6" s="59">
-        <v>15</v>
-      </c>
-      <c r="F6" s="18">
-        <v>15</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="B6" s="55">
+        <v>15</v>
+      </c>
+      <c r="C6" s="55">
+        <v>15</v>
+      </c>
+      <c r="D6" s="55">
+        <v>15</v>
+      </c>
+      <c r="E6" s="55">
+        <v>15</v>
+      </c>
+      <c r="F6" s="49">
+        <v>15</v>
+      </c>
+      <c r="G6" s="49">
         <v>8</v>
       </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
+      <c r="H6" s="49">
+        <v>0</v>
+      </c>
+      <c r="I6" s="18">
+        <v>3</v>
+      </c>
       <c r="J6" s="49"/>
       <c r="K6" s="49"/>
       <c r="L6" s="49"/>
@@ -1283,7 +1303,7 @@
       <c r="U6" s="49"/>
       <c r="V6" s="39">
         <f t="shared" si="0"/>
-        <v>0.92222222222222228</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="W6"/>
     </row>
@@ -1291,26 +1311,30 @@
       <c r="A7" s="29">
         <v>1395</v>
       </c>
-      <c r="B7" s="59">
-        <v>15</v>
-      </c>
-      <c r="C7" s="59">
-        <v>15</v>
-      </c>
-      <c r="D7" s="59">
+      <c r="B7" s="55">
+        <v>15</v>
+      </c>
+      <c r="C7" s="55">
+        <v>15</v>
+      </c>
+      <c r="D7" s="55">
         <v>9</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="55">
         <v>13</v>
       </c>
-      <c r="F7" s="18">
-        <v>15</v>
-      </c>
-      <c r="G7" s="18">
+      <c r="F7" s="49">
+        <v>15</v>
+      </c>
+      <c r="G7" s="49">
         <v>12</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
+      <c r="H7" s="49">
+        <v>3</v>
+      </c>
+      <c r="I7" s="18">
+        <v>3</v>
+      </c>
       <c r="J7" s="49"/>
       <c r="K7" s="49"/>
       <c r="L7" s="49"/>
@@ -1325,7 +1349,7 @@
       <c r="U7" s="49"/>
       <c r="V7" s="39">
         <f t="shared" si="0"/>
-        <v>0.87777777777777777</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="W7"/>
     </row>
@@ -1333,26 +1357,30 @@
       <c r="A8" s="29">
         <v>1506</v>
       </c>
-      <c r="B8" s="59">
-        <v>15</v>
-      </c>
-      <c r="C8" s="59">
-        <v>15</v>
-      </c>
-      <c r="D8" s="59">
-        <v>3</v>
-      </c>
-      <c r="E8" s="59">
-        <v>3</v>
-      </c>
-      <c r="F8" s="18">
-        <v>3</v>
-      </c>
-      <c r="G8" s="18">
-        <v>3</v>
-      </c>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
+      <c r="B8" s="55">
+        <v>15</v>
+      </c>
+      <c r="C8" s="55">
+        <v>15</v>
+      </c>
+      <c r="D8" s="55">
+        <v>3</v>
+      </c>
+      <c r="E8" s="55">
+        <v>3</v>
+      </c>
+      <c r="F8" s="49">
+        <v>3</v>
+      </c>
+      <c r="G8" s="49">
+        <v>3</v>
+      </c>
+      <c r="H8" s="49">
+        <v>3</v>
+      </c>
+      <c r="I8" s="18">
+        <v>3</v>
+      </c>
       <c r="J8" s="49"/>
       <c r="K8" s="49"/>
       <c r="L8" s="49"/>
@@ -1367,7 +1395,7 @@
       <c r="U8" s="49"/>
       <c r="V8" s="39">
         <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="W8"/>
     </row>
@@ -1375,26 +1403,30 @@
       <c r="A9" s="29">
         <v>2441</v>
       </c>
-      <c r="B9" s="59">
-        <v>15</v>
-      </c>
-      <c r="C9" s="59">
-        <v>0</v>
-      </c>
-      <c r="D9" s="59">
-        <v>3</v>
-      </c>
-      <c r="E9" s="59">
-        <v>0</v>
-      </c>
-      <c r="F9" s="18">
-        <v>3</v>
-      </c>
-      <c r="G9" s="18">
-        <v>3</v>
-      </c>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
+      <c r="B9" s="55">
+        <v>15</v>
+      </c>
+      <c r="C9" s="55">
+        <v>0</v>
+      </c>
+      <c r="D9" s="55">
+        <v>3</v>
+      </c>
+      <c r="E9" s="55">
+        <v>0</v>
+      </c>
+      <c r="F9" s="49">
+        <v>3</v>
+      </c>
+      <c r="G9" s="49">
+        <v>3</v>
+      </c>
+      <c r="H9" s="49">
+        <v>0</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
       <c r="J9" s="49"/>
       <c r="K9" s="49"/>
       <c r="L9" s="49"/>
@@ -1409,7 +1441,7 @@
       <c r="U9" s="49"/>
       <c r="V9" s="39">
         <f t="shared" si="0"/>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
       <c r="W9"/>
     </row>
@@ -1417,26 +1449,28 @@
       <c r="A10" s="29">
         <v>2564</v>
       </c>
-      <c r="B10" s="59">
-        <v>15</v>
-      </c>
-      <c r="C10" s="59">
-        <v>15</v>
-      </c>
-      <c r="D10" s="59">
-        <v>3</v>
-      </c>
-      <c r="E10" s="59">
-        <v>15</v>
-      </c>
-      <c r="F10" s="18">
-        <v>3</v>
-      </c>
-      <c r="G10" s="18">
+      <c r="B10" s="55">
+        <v>15</v>
+      </c>
+      <c r="C10" s="55">
+        <v>15</v>
+      </c>
+      <c r="D10" s="55">
+        <v>3</v>
+      </c>
+      <c r="E10" s="55">
+        <v>15</v>
+      </c>
+      <c r="F10" s="49">
+        <v>3</v>
+      </c>
+      <c r="G10" s="49">
         <v>15</v>
       </c>
       <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
+      <c r="I10" s="18">
+        <v>3</v>
+      </c>
       <c r="J10" s="49"/>
       <c r="K10" s="49"/>
       <c r="L10" s="49"/>
@@ -1451,7 +1485,7 @@
       <c r="U10" s="49"/>
       <c r="V10" s="39">
         <f t="shared" si="0"/>
-        <v>0.73333333333333328</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="W10"/>
     </row>
@@ -1459,26 +1493,30 @@
       <c r="A11" s="29">
         <v>2693</v>
       </c>
-      <c r="B11" s="59">
-        <v>0</v>
-      </c>
-      <c r="C11" s="59">
-        <v>0</v>
-      </c>
-      <c r="D11" s="59">
-        <v>0</v>
-      </c>
-      <c r="E11" s="59">
-        <v>0</v>
-      </c>
-      <c r="F11" s="18">
-        <v>0</v>
-      </c>
-      <c r="G11" s="18">
-        <v>0</v>
-      </c>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
+      <c r="B11" s="55">
+        <v>0</v>
+      </c>
+      <c r="C11" s="55">
+        <v>0</v>
+      </c>
+      <c r="D11" s="55">
+        <v>0</v>
+      </c>
+      <c r="E11" s="55">
+        <v>0</v>
+      </c>
+      <c r="F11" s="49">
+        <v>0</v>
+      </c>
+      <c r="G11" s="49">
+        <v>0</v>
+      </c>
+      <c r="H11" s="49">
+        <v>0</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0</v>
+      </c>
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
       <c r="L11" s="49"/>
@@ -1501,26 +1539,30 @@
       <c r="A12" s="29">
         <v>2771</v>
       </c>
-      <c r="B12" s="59">
-        <v>0</v>
-      </c>
-      <c r="C12" s="59">
-        <v>0</v>
-      </c>
-      <c r="D12" s="59">
-        <v>3</v>
-      </c>
-      <c r="E12" s="59">
-        <v>0</v>
-      </c>
-      <c r="F12" s="18">
-        <v>3</v>
-      </c>
-      <c r="G12" s="18">
-        <v>0</v>
-      </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
+      <c r="B12" s="55">
+        <v>0</v>
+      </c>
+      <c r="C12" s="55">
+        <v>0</v>
+      </c>
+      <c r="D12" s="55">
+        <v>3</v>
+      </c>
+      <c r="E12" s="55">
+        <v>0</v>
+      </c>
+      <c r="F12" s="49">
+        <v>3</v>
+      </c>
+      <c r="G12" s="49">
+        <v>0</v>
+      </c>
+      <c r="H12" s="49">
+        <v>0</v>
+      </c>
+      <c r="I12" s="18">
+        <v>0</v>
+      </c>
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
@@ -1535,7 +1577,7 @@
       <c r="U12" s="49"/>
       <c r="V12" s="39">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+        <v>0.05</v>
       </c>
       <c r="W12"/>
     </row>
@@ -1543,26 +1585,30 @@
       <c r="A13" s="29">
         <v>2899</v>
       </c>
-      <c r="B13" s="59">
-        <v>15</v>
-      </c>
-      <c r="C13" s="59">
-        <v>15</v>
-      </c>
-      <c r="D13" s="59">
-        <v>0</v>
-      </c>
-      <c r="E13" s="59">
-        <v>3</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
+      <c r="B13" s="55">
+        <v>15</v>
+      </c>
+      <c r="C13" s="55">
+        <v>15</v>
+      </c>
+      <c r="D13" s="55">
+        <v>0</v>
+      </c>
+      <c r="E13" s="55">
+        <v>3</v>
+      </c>
+      <c r="F13" s="49">
+        <v>0</v>
+      </c>
+      <c r="G13" s="49">
+        <v>0</v>
+      </c>
+      <c r="H13" s="49">
+        <v>3</v>
+      </c>
+      <c r="I13" s="18">
+        <v>0</v>
+      </c>
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
       <c r="L13" s="49"/>
@@ -1577,7 +1623,7 @@
       <c r="U13" s="49"/>
       <c r="V13" s="39">
         <f t="shared" si="0"/>
-        <v>0.36666666666666664</v>
+        <v>0.3</v>
       </c>
       <c r="W13"/>
     </row>
@@ -1585,26 +1631,30 @@
       <c r="A14" s="29">
         <v>3517</v>
       </c>
-      <c r="B14" s="59">
-        <v>15</v>
-      </c>
-      <c r="C14" s="59">
-        <v>15</v>
-      </c>
-      <c r="D14" s="59">
-        <v>3</v>
-      </c>
-      <c r="E14" s="59">
-        <v>3</v>
-      </c>
-      <c r="F14" s="18">
-        <v>0</v>
-      </c>
-      <c r="G14" s="18">
-        <v>15</v>
-      </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
+      <c r="B14" s="55">
+        <v>15</v>
+      </c>
+      <c r="C14" s="55">
+        <v>15</v>
+      </c>
+      <c r="D14" s="55">
+        <v>3</v>
+      </c>
+      <c r="E14" s="55">
+        <v>3</v>
+      </c>
+      <c r="F14" s="49">
+        <v>0</v>
+      </c>
+      <c r="G14" s="49">
+        <v>15</v>
+      </c>
+      <c r="H14" s="49">
+        <v>3</v>
+      </c>
+      <c r="I14" s="18">
+        <v>3</v>
+      </c>
       <c r="J14" s="49"/>
       <c r="K14" s="49"/>
       <c r="L14" s="49"/>
@@ -1619,33 +1669,37 @@
       <c r="U14" s="49"/>
       <c r="V14" s="39">
         <f t="shared" si="0"/>
-        <v>0.56666666666666665</v>
+        <v>0.47499999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="29">
         <v>4490</v>
       </c>
-      <c r="B15" s="59">
-        <v>15</v>
-      </c>
-      <c r="C15" s="59">
-        <v>15</v>
-      </c>
-      <c r="D15" s="59">
-        <v>15</v>
-      </c>
-      <c r="E15" s="59">
-        <v>15</v>
-      </c>
-      <c r="F15" s="18">
-        <v>15</v>
-      </c>
-      <c r="G15" s="18">
-        <v>15</v>
-      </c>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
+      <c r="B15" s="55">
+        <v>15</v>
+      </c>
+      <c r="C15" s="55">
+        <v>15</v>
+      </c>
+      <c r="D15" s="55">
+        <v>15</v>
+      </c>
+      <c r="E15" s="55">
+        <v>15</v>
+      </c>
+      <c r="F15" s="49">
+        <v>15</v>
+      </c>
+      <c r="G15" s="49">
+        <v>15</v>
+      </c>
+      <c r="H15" s="49">
+        <v>3</v>
+      </c>
+      <c r="I15" s="18">
+        <v>6</v>
+      </c>
       <c r="J15" s="49"/>
       <c r="K15" s="49"/>
       <c r="L15" s="49"/>
@@ -1660,7 +1714,7 @@
       <c r="U15" s="49"/>
       <c r="V15" s="39">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="W15"/>
     </row>
@@ -1668,26 +1722,30 @@
       <c r="A16" s="29">
         <v>4582</v>
       </c>
-      <c r="B16" s="59">
-        <v>15</v>
-      </c>
-      <c r="C16" s="59">
-        <v>15</v>
-      </c>
-      <c r="D16" s="59">
-        <v>3</v>
-      </c>
-      <c r="E16" s="59">
+      <c r="B16" s="55">
+        <v>15</v>
+      </c>
+      <c r="C16" s="55">
+        <v>15</v>
+      </c>
+      <c r="D16" s="55">
+        <v>3</v>
+      </c>
+      <c r="E16" s="55">
         <v>10</v>
       </c>
-      <c r="F16" s="18">
-        <v>15</v>
-      </c>
-      <c r="G16" s="18">
+      <c r="F16" s="49">
+        <v>15</v>
+      </c>
+      <c r="G16" s="49">
         <v>8</v>
       </c>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
+      <c r="H16" s="49">
+        <v>3</v>
+      </c>
+      <c r="I16" s="18">
+        <v>3</v>
+      </c>
       <c r="J16" s="49"/>
       <c r="K16" s="49"/>
       <c r="L16" s="49"/>
@@ -1702,7 +1760,7 @@
       <c r="U16" s="49"/>
       <c r="V16" s="39">
         <f t="shared" si="0"/>
-        <v>0.73333333333333328</v>
+        <v>0.6</v>
       </c>
       <c r="W16"/>
     </row>
@@ -1710,26 +1768,30 @@
       <c r="A17" s="29">
         <v>4622</v>
       </c>
-      <c r="B17" s="59">
-        <v>15</v>
-      </c>
-      <c r="C17" s="59">
-        <v>15</v>
-      </c>
-      <c r="D17" s="59">
+      <c r="B17" s="55">
+        <v>15</v>
+      </c>
+      <c r="C17" s="55">
+        <v>15</v>
+      </c>
+      <c r="D17" s="55">
         <v>12</v>
       </c>
-      <c r="E17" s="59">
+      <c r="E17" s="55">
         <v>8</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="49">
         <v>12</v>
       </c>
-      <c r="G17" s="18">
-        <v>3</v>
-      </c>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="G17" s="49">
+        <v>3</v>
+      </c>
+      <c r="H17" s="49">
+        <v>12</v>
+      </c>
+      <c r="I17" s="18">
+        <v>3</v>
+      </c>
       <c r="J17" s="49"/>
       <c r="K17" s="49"/>
       <c r="L17" s="49"/>
@@ -1744,7 +1806,7 @@
       <c r="U17" s="49"/>
       <c r="V17" s="39">
         <f t="shared" si="0"/>
-        <v>0.72222222222222221</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="W17"/>
     </row>
@@ -1752,26 +1814,30 @@
       <c r="A18" s="29">
         <v>5500</v>
       </c>
-      <c r="B18" s="59">
-        <v>15</v>
-      </c>
-      <c r="C18" s="59">
-        <v>15</v>
-      </c>
-      <c r="D18" s="59">
-        <v>3</v>
-      </c>
-      <c r="E18" s="59">
+      <c r="B18" s="55">
+        <v>15</v>
+      </c>
+      <c r="C18" s="55">
+        <v>15</v>
+      </c>
+      <c r="D18" s="55">
+        <v>3</v>
+      </c>
+      <c r="E18" s="55">
         <v>12</v>
       </c>
-      <c r="F18" s="18">
-        <v>3</v>
-      </c>
-      <c r="G18" s="18">
-        <v>15</v>
-      </c>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
+      <c r="F18" s="49">
+        <v>3</v>
+      </c>
+      <c r="G18" s="49">
+        <v>15</v>
+      </c>
+      <c r="H18" s="49">
+        <v>3</v>
+      </c>
+      <c r="I18" s="18">
+        <v>3</v>
+      </c>
       <c r="J18" s="49"/>
       <c r="K18" s="49"/>
       <c r="L18" s="49"/>
@@ -1786,7 +1852,7 @@
       <c r="U18" s="49"/>
       <c r="V18" s="39">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="W18"/>
     </row>
@@ -1794,26 +1860,30 @@
       <c r="A19" s="29">
         <v>5687</v>
       </c>
-      <c r="B19" s="59">
-        <v>15</v>
-      </c>
-      <c r="C19" s="59">
-        <v>15</v>
-      </c>
-      <c r="D19" s="59">
-        <v>0</v>
-      </c>
-      <c r="E19" s="59">
-        <v>15</v>
-      </c>
-      <c r="F19" s="18">
-        <v>3</v>
-      </c>
-      <c r="G19" s="18">
+      <c r="B19" s="55">
+        <v>15</v>
+      </c>
+      <c r="C19" s="55">
+        <v>15</v>
+      </c>
+      <c r="D19" s="55">
+        <v>0</v>
+      </c>
+      <c r="E19" s="55">
+        <v>15</v>
+      </c>
+      <c r="F19" s="49">
+        <v>3</v>
+      </c>
+      <c r="G19" s="49">
         <v>12</v>
       </c>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
+      <c r="H19" s="49">
+        <v>3</v>
+      </c>
+      <c r="I19" s="18">
+        <v>3</v>
+      </c>
       <c r="J19" s="49"/>
       <c r="K19" s="49"/>
       <c r="L19" s="49"/>
@@ -1828,7 +1898,7 @@
       <c r="U19" s="49"/>
       <c r="V19" s="39">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W19"/>
     </row>
@@ -1836,26 +1906,30 @@
       <c r="A20" s="29">
         <v>5711</v>
       </c>
-      <c r="B20" s="59">
-        <v>15</v>
-      </c>
-      <c r="C20" s="59">
-        <v>15</v>
-      </c>
-      <c r="D20" s="59">
-        <v>3</v>
-      </c>
-      <c r="E20" s="59">
-        <v>3</v>
-      </c>
-      <c r="F20" s="18">
-        <v>0</v>
-      </c>
-      <c r="G20" s="18">
-        <v>3</v>
-      </c>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
+      <c r="B20" s="55">
+        <v>15</v>
+      </c>
+      <c r="C20" s="55">
+        <v>15</v>
+      </c>
+      <c r="D20" s="55">
+        <v>3</v>
+      </c>
+      <c r="E20" s="55">
+        <v>3</v>
+      </c>
+      <c r="F20" s="49">
+        <v>0</v>
+      </c>
+      <c r="G20" s="49">
+        <v>3</v>
+      </c>
+      <c r="H20" s="49">
+        <v>3</v>
+      </c>
+      <c r="I20" s="18">
+        <v>0</v>
+      </c>
       <c r="J20" s="49"/>
       <c r="K20" s="49"/>
       <c r="L20" s="49"/>
@@ -1870,7 +1944,7 @@
       <c r="U20" s="49"/>
       <c r="V20" s="39">
         <f t="shared" si="0"/>
-        <v>0.43333333333333335</v>
+        <v>0.35</v>
       </c>
       <c r="W20"/>
     </row>
@@ -1878,26 +1952,30 @@
       <c r="A21" s="29">
         <v>5810</v>
       </c>
-      <c r="B21" s="59">
-        <v>15</v>
-      </c>
-      <c r="C21" s="59">
-        <v>15</v>
-      </c>
-      <c r="D21" s="59">
+      <c r="B21" s="55">
+        <v>15</v>
+      </c>
+      <c r="C21" s="55">
+        <v>15</v>
+      </c>
+      <c r="D21" s="55">
         <v>12</v>
       </c>
-      <c r="E21" s="59">
+      <c r="E21" s="55">
         <v>12</v>
       </c>
-      <c r="F21" s="18">
-        <v>3</v>
-      </c>
-      <c r="G21" s="18">
-        <v>15</v>
-      </c>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
+      <c r="F21" s="49">
+        <v>3</v>
+      </c>
+      <c r="G21" s="49">
+        <v>15</v>
+      </c>
+      <c r="H21" s="49">
+        <v>3</v>
+      </c>
+      <c r="I21" s="18">
+        <v>3</v>
+      </c>
       <c r="J21" s="49"/>
       <c r="K21" s="49"/>
       <c r="L21" s="49"/>
@@ -1912,7 +1990,7 @@
       <c r="U21" s="49"/>
       <c r="V21" s="39">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W21"/>
     </row>
@@ -1920,26 +1998,30 @@
       <c r="A22" s="29">
         <v>6347</v>
       </c>
-      <c r="B22" s="59">
-        <v>15</v>
-      </c>
-      <c r="C22" s="59">
-        <v>15</v>
-      </c>
-      <c r="D22" s="59">
-        <v>3</v>
-      </c>
-      <c r="E22" s="59">
+      <c r="B22" s="55">
+        <v>15</v>
+      </c>
+      <c r="C22" s="55">
+        <v>15</v>
+      </c>
+      <c r="D22" s="55">
+        <v>3</v>
+      </c>
+      <c r="E22" s="55">
         <v>12</v>
       </c>
-      <c r="F22" s="18">
-        <v>15</v>
-      </c>
-      <c r="G22" s="18">
+      <c r="F22" s="49">
+        <v>15</v>
+      </c>
+      <c r="G22" s="49">
         <v>8</v>
       </c>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
+      <c r="H22" s="49">
+        <v>3</v>
+      </c>
+      <c r="I22" s="18">
+        <v>3</v>
+      </c>
       <c r="J22" s="49"/>
       <c r="K22" s="49"/>
       <c r="L22" s="49"/>
@@ -1954,7 +2036,7 @@
       <c r="U22" s="49"/>
       <c r="V22" s="39">
         <f t="shared" si="0"/>
-        <v>0.75555555555555554</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="W22"/>
     </row>
@@ -1962,26 +2044,30 @@
       <c r="A23" s="29">
         <v>7905</v>
       </c>
-      <c r="B23" s="59">
-        <v>15</v>
-      </c>
-      <c r="C23" s="59">
-        <v>15</v>
-      </c>
-      <c r="D23" s="59">
+      <c r="B23" s="55">
+        <v>15</v>
+      </c>
+      <c r="C23" s="55">
+        <v>15</v>
+      </c>
+      <c r="D23" s="55">
         <v>12</v>
       </c>
-      <c r="E23" s="59">
-        <v>3</v>
-      </c>
-      <c r="F23" s="18">
-        <v>3</v>
-      </c>
-      <c r="G23" s="18">
-        <v>0</v>
-      </c>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
+      <c r="E23" s="55">
+        <v>3</v>
+      </c>
+      <c r="F23" s="49">
+        <v>3</v>
+      </c>
+      <c r="G23" s="49">
+        <v>0</v>
+      </c>
+      <c r="H23" s="49">
+        <v>3</v>
+      </c>
+      <c r="I23" s="18">
+        <v>3</v>
+      </c>
       <c r="J23" s="49"/>
       <c r="K23" s="49"/>
       <c r="L23" s="49"/>
@@ -1996,7 +2082,7 @@
       <c r="U23" s="49"/>
       <c r="V23" s="39">
         <f t="shared" si="0"/>
-        <v>0.53333333333333333</v>
+        <v>0.45</v>
       </c>
       <c r="W23"/>
     </row>
@@ -2004,26 +2090,30 @@
       <c r="A24" s="29">
         <v>8335</v>
       </c>
-      <c r="B24" s="59">
-        <v>15</v>
-      </c>
-      <c r="C24" s="59">
-        <v>15</v>
-      </c>
-      <c r="D24" s="59">
-        <v>3</v>
-      </c>
-      <c r="E24" s="59">
+      <c r="B24" s="55">
+        <v>15</v>
+      </c>
+      <c r="C24" s="55">
+        <v>15</v>
+      </c>
+      <c r="D24" s="55">
+        <v>3</v>
+      </c>
+      <c r="E24" s="55">
         <v>12</v>
       </c>
-      <c r="F24" s="18">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18">
-        <v>3</v>
-      </c>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
+      <c r="F24" s="49">
+        <v>0</v>
+      </c>
+      <c r="G24" s="49">
+        <v>3</v>
+      </c>
+      <c r="H24" s="49">
+        <v>0</v>
+      </c>
+      <c r="I24" s="18">
+        <v>0</v>
+      </c>
       <c r="J24" s="49"/>
       <c r="K24" s="49"/>
       <c r="L24" s="49"/>
@@ -2038,7 +2128,7 @@
       <c r="U24" s="49"/>
       <c r="V24" s="39">
         <f t="shared" si="0"/>
-        <v>0.53333333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="W24"/>
     </row>
@@ -2046,26 +2136,30 @@
       <c r="A25" s="29">
         <v>8490</v>
       </c>
-      <c r="B25" s="59">
-        <v>3</v>
-      </c>
-      <c r="C25" s="59">
-        <v>15</v>
-      </c>
-      <c r="D25" s="59">
+      <c r="B25" s="55">
+        <v>3</v>
+      </c>
+      <c r="C25" s="55">
+        <v>15</v>
+      </c>
+      <c r="D25" s="55">
         <v>12</v>
       </c>
-      <c r="E25" s="59">
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <v>3</v>
-      </c>
-      <c r="G25" s="18">
+      <c r="E25" s="55">
+        <v>0</v>
+      </c>
+      <c r="F25" s="49">
+        <v>3</v>
+      </c>
+      <c r="G25" s="49">
         <v>12</v>
       </c>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
+      <c r="H25" s="49">
+        <v>3</v>
+      </c>
+      <c r="I25" s="18">
+        <v>3</v>
+      </c>
       <c r="J25" s="49"/>
       <c r="K25" s="49"/>
       <c r="L25" s="49"/>
@@ -2080,7 +2174,7 @@
       <c r="U25" s="49"/>
       <c r="V25" s="39">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="W25"/>
     </row>
@@ -2088,26 +2182,30 @@
       <c r="A26" s="29">
         <v>8688</v>
       </c>
-      <c r="B26" s="59">
-        <v>15</v>
-      </c>
-      <c r="C26" s="59">
-        <v>0</v>
-      </c>
-      <c r="D26" s="59">
-        <v>15</v>
-      </c>
-      <c r="E26" s="59">
-        <v>0</v>
-      </c>
-      <c r="F26" s="18">
-        <v>15</v>
-      </c>
-      <c r="G26" s="18">
-        <v>3</v>
-      </c>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
+      <c r="B26" s="55">
+        <v>15</v>
+      </c>
+      <c r="C26" s="55">
+        <v>0</v>
+      </c>
+      <c r="D26" s="55">
+        <v>15</v>
+      </c>
+      <c r="E26" s="55">
+        <v>0</v>
+      </c>
+      <c r="F26" s="49">
+        <v>15</v>
+      </c>
+      <c r="G26" s="49">
+        <v>3</v>
+      </c>
+      <c r="H26" s="49">
+        <v>3</v>
+      </c>
+      <c r="I26" s="18">
+        <v>15</v>
+      </c>
       <c r="J26" s="49"/>
       <c r="K26" s="49"/>
       <c r="L26" s="49"/>
@@ -2122,7 +2220,7 @@
       <c r="U26" s="49"/>
       <c r="V26" s="39">
         <f t="shared" si="0"/>
-        <v>0.53333333333333333</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W26"/>
     </row>
@@ -2130,26 +2228,30 @@
       <c r="A27" s="29">
         <v>8695</v>
       </c>
-      <c r="B27" s="59">
-        <v>15</v>
-      </c>
-      <c r="C27" s="59">
-        <v>15</v>
-      </c>
-      <c r="D27" s="59">
-        <v>3</v>
-      </c>
-      <c r="E27" s="59">
-        <v>15</v>
-      </c>
-      <c r="F27" s="18">
-        <v>3</v>
-      </c>
-      <c r="G27" s="18">
+      <c r="B27" s="55">
+        <v>15</v>
+      </c>
+      <c r="C27" s="55">
+        <v>15</v>
+      </c>
+      <c r="D27" s="55">
+        <v>3</v>
+      </c>
+      <c r="E27" s="55">
+        <v>15</v>
+      </c>
+      <c r="F27" s="49">
+        <v>3</v>
+      </c>
+      <c r="G27" s="49">
         <v>8</v>
       </c>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
+      <c r="H27" s="49">
+        <v>3</v>
+      </c>
+      <c r="I27" s="18">
+        <v>3</v>
+      </c>
       <c r="J27" s="49"/>
       <c r="K27" s="49"/>
       <c r="L27" s="49"/>
@@ -2164,7 +2266,7 @@
       <c r="U27" s="49"/>
       <c r="V27" s="39">
         <f t="shared" si="0"/>
-        <v>0.65555555555555556</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="W27"/>
     </row>
@@ -2172,26 +2274,30 @@
       <c r="A28" s="29">
         <v>8743</v>
       </c>
-      <c r="B28" s="59">
-        <v>15</v>
-      </c>
-      <c r="C28" s="59">
-        <v>15</v>
-      </c>
-      <c r="D28" s="59">
-        <v>3</v>
-      </c>
-      <c r="E28" s="59">
-        <v>3</v>
-      </c>
-      <c r="F28" s="18">
-        <v>3</v>
-      </c>
-      <c r="G28" s="18">
-        <v>3</v>
-      </c>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
+      <c r="B28" s="55">
+        <v>15</v>
+      </c>
+      <c r="C28" s="55">
+        <v>15</v>
+      </c>
+      <c r="D28" s="55">
+        <v>3</v>
+      </c>
+      <c r="E28" s="55">
+        <v>3</v>
+      </c>
+      <c r="F28" s="49">
+        <v>3</v>
+      </c>
+      <c r="G28" s="49">
+        <v>3</v>
+      </c>
+      <c r="H28" s="49">
+        <v>3</v>
+      </c>
+      <c r="I28" s="18">
+        <v>3</v>
+      </c>
       <c r="J28" s="49"/>
       <c r="K28" s="49"/>
       <c r="L28" s="49"/>
@@ -2206,7 +2312,7 @@
       <c r="U28" s="49"/>
       <c r="V28" s="39">
         <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="W28"/>
     </row>
@@ -2214,26 +2320,28 @@
       <c r="A29" s="29">
         <v>8745</v>
       </c>
-      <c r="B29" s="59">
-        <v>15</v>
-      </c>
-      <c r="C29" s="59">
-        <v>15</v>
-      </c>
-      <c r="D29" s="59">
+      <c r="B29" s="55">
+        <v>15</v>
+      </c>
+      <c r="C29" s="55">
+        <v>15</v>
+      </c>
+      <c r="D29" s="55">
         <v>12</v>
       </c>
-      <c r="E29" s="59">
-        <v>15</v>
-      </c>
-      <c r="F29" s="18">
-        <v>3</v>
-      </c>
-      <c r="G29" s="18">
-        <v>3</v>
-      </c>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
+      <c r="E29" s="55">
+        <v>15</v>
+      </c>
+      <c r="F29" s="49">
+        <v>3</v>
+      </c>
+      <c r="G29" s="49">
+        <v>3</v>
+      </c>
+      <c r="H29" s="59"/>
+      <c r="I29" s="18">
+        <v>3</v>
+      </c>
       <c r="J29" s="49"/>
       <c r="K29" s="49"/>
       <c r="L29" s="49"/>
@@ -2248,7 +2356,7 @@
       <c r="U29" s="49"/>
       <c r="V29" s="39">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W29"/>
     </row>
@@ -2256,26 +2364,30 @@
       <c r="A30" s="29">
         <v>9550</v>
       </c>
-      <c r="B30" s="59">
-        <v>15</v>
-      </c>
-      <c r="C30" s="59">
-        <v>15</v>
-      </c>
-      <c r="D30" s="59">
-        <v>3</v>
-      </c>
-      <c r="E30" s="59">
-        <v>3</v>
-      </c>
-      <c r="F30" s="18">
-        <v>3</v>
-      </c>
-      <c r="G30" s="18">
-        <v>3</v>
-      </c>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
+      <c r="B30" s="55">
+        <v>15</v>
+      </c>
+      <c r="C30" s="55">
+        <v>15</v>
+      </c>
+      <c r="D30" s="55">
+        <v>3</v>
+      </c>
+      <c r="E30" s="55">
+        <v>3</v>
+      </c>
+      <c r="F30" s="49">
+        <v>3</v>
+      </c>
+      <c r="G30" s="49">
+        <v>3</v>
+      </c>
+      <c r="H30" s="49">
+        <v>3</v>
+      </c>
+      <c r="I30" s="18">
+        <v>3</v>
+      </c>
       <c r="J30" s="49"/>
       <c r="K30" s="49"/>
       <c r="L30" s="49"/>
@@ -2290,7 +2402,7 @@
       <c r="U30" s="49"/>
       <c r="V30" s="39">
         <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="W30"/>
     </row>
@@ -2298,26 +2410,30 @@
       <c r="A31" s="29">
         <v>9610</v>
       </c>
-      <c r="B31" s="59">
-        <v>15</v>
-      </c>
-      <c r="C31" s="59">
-        <v>15</v>
-      </c>
-      <c r="D31" s="59">
-        <v>3</v>
-      </c>
-      <c r="E31" s="59">
-        <v>3</v>
-      </c>
-      <c r="F31" s="18">
-        <v>3</v>
-      </c>
-      <c r="G31" s="18">
-        <v>3</v>
-      </c>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
+      <c r="B31" s="55">
+        <v>15</v>
+      </c>
+      <c r="C31" s="55">
+        <v>15</v>
+      </c>
+      <c r="D31" s="55">
+        <v>3</v>
+      </c>
+      <c r="E31" s="55">
+        <v>3</v>
+      </c>
+      <c r="F31" s="49">
+        <v>3</v>
+      </c>
+      <c r="G31" s="49">
+        <v>3</v>
+      </c>
+      <c r="H31" s="49">
+        <v>3</v>
+      </c>
+      <c r="I31" s="18">
+        <v>3</v>
+      </c>
       <c r="J31" s="49"/>
       <c r="K31" s="49"/>
       <c r="L31" s="49"/>
@@ -2332,7 +2448,7 @@
       <c r="U31" s="49"/>
       <c r="V31" s="39">
         <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="W31"/>
     </row>
@@ -2340,26 +2456,30 @@
       <c r="A32" s="29">
         <v>9611</v>
       </c>
-      <c r="B32" s="59">
-        <v>15</v>
-      </c>
-      <c r="C32" s="59">
-        <v>15</v>
-      </c>
-      <c r="D32" s="59">
-        <v>3</v>
-      </c>
-      <c r="E32" s="59">
-        <v>3</v>
-      </c>
-      <c r="F32" s="18">
-        <v>3</v>
-      </c>
-      <c r="G32" s="18">
-        <v>3</v>
-      </c>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
+      <c r="B32" s="55">
+        <v>15</v>
+      </c>
+      <c r="C32" s="55">
+        <v>15</v>
+      </c>
+      <c r="D32" s="55">
+        <v>3</v>
+      </c>
+      <c r="E32" s="55">
+        <v>3</v>
+      </c>
+      <c r="F32" s="49">
+        <v>3</v>
+      </c>
+      <c r="G32" s="49">
+        <v>3</v>
+      </c>
+      <c r="H32" s="49">
+        <v>3</v>
+      </c>
+      <c r="I32" s="18">
+        <v>3</v>
+      </c>
       <c r="J32" s="49"/>
       <c r="K32" s="49"/>
       <c r="L32" s="49"/>
@@ -2374,7 +2494,7 @@
       <c r="U32" s="49"/>
       <c r="V32" s="39">
         <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="W32"/>
     </row>
@@ -2382,26 +2502,30 @@
       <c r="A33" s="29">
         <v>9674</v>
       </c>
-      <c r="B33" s="59">
-        <v>15</v>
-      </c>
-      <c r="C33" s="59">
-        <v>15</v>
-      </c>
-      <c r="D33" s="59">
+      <c r="B33" s="55">
+        <v>15</v>
+      </c>
+      <c r="C33" s="55">
+        <v>15</v>
+      </c>
+      <c r="D33" s="55">
         <v>8</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="55">
         <v>12</v>
       </c>
-      <c r="F33" s="18">
-        <v>3</v>
-      </c>
-      <c r="G33" s="18">
-        <v>15</v>
-      </c>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
+      <c r="F33" s="49">
+        <v>3</v>
+      </c>
+      <c r="G33" s="49">
+        <v>15</v>
+      </c>
+      <c r="H33" s="49">
+        <v>3</v>
+      </c>
+      <c r="I33" s="18">
+        <v>3</v>
+      </c>
       <c r="J33" s="49"/>
       <c r="K33" s="49"/>
       <c r="L33" s="49"/>
@@ -2416,7 +2540,7 @@
       <c r="U33" s="49"/>
       <c r="V33" s="39">
         <f t="shared" si="0"/>
-        <v>0.75555555555555554</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="W33"/>
     </row>
@@ -2542,13 +2666,13 @@
         <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
-      <c r="H36" s="35" t="e">
+      <c r="H36" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I36" s="35" t="e">
+        <v>2.8666666666666667</v>
+      </c>
+      <c r="I36" s="35">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2.8125</v>
       </c>
       <c r="J36" s="35" t="e">
         <f t="shared" si="1"/>
@@ -2600,7 +2724,7 @@
       </c>
       <c r="V36" s="35">
         <f t="shared" si="1"/>
-        <v>0.5586805555555554</v>
+        <v>0.46484375000000011</v>
       </c>
       <c r="W36"/>
     </row>
@@ -2632,13 +2756,13 @@
         <f t="shared" si="2"/>
         <v>5.4299052448216756</v>
       </c>
-      <c r="H37" s="35" t="e">
+      <c r="H37" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I37" s="35" t="e">
+        <v>2.3449628088122516</v>
+      </c>
+      <c r="I37" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>2.6327650128530702</v>
       </c>
       <c r="J37" s="35" t="e">
         <f t="shared" si="2"/>
@@ -2690,7 +2814,7 @@
       </c>
       <c r="V37" s="35">
         <f t="shared" si="2"/>
-        <v>0.24232108690680965</v>
+        <v>0.19930136012094168</v>
       </c>
       <c r="W37"/>
     </row>
@@ -2722,13 +2846,13 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="H38" s="35" t="e">
+      <c r="H38" s="35">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I38" s="35" t="e">
+        <v>3</v>
+      </c>
+      <c r="I38" s="35">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>3</v>
       </c>
       <c r="J38" s="35" t="e">
         <f t="shared" si="3"/>
@@ -2780,7 +2904,7 @@
       </c>
       <c r="V38" s="35">
         <f t="shared" si="3"/>
-        <v>0.53333333333333333</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="W38"/>
     </row>
@@ -2814,11 +2938,11 @@
       </c>
       <c r="H39" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="38">
         <f t="shared" si="4"/>
@@ -4762,7 +4886,7 @@
       </c>
       <c r="B2" s="21">
         <f>Quiz!V2</f>
-        <v>0.43333333333333335</v>
+        <v>0.375</v>
       </c>
       <c r="C2" s="20">
         <f>Homework!L2</f>
@@ -4778,7 +4902,7 @@
       </c>
       <c r="F2" s="21">
         <f t="shared" ref="F2:F17" si="0">$B2+$C2+($D2/$D$35)*3+($E2/$E$35)*4.5</f>
-        <v>0.43333333333333335</v>
+        <v>0.375</v>
       </c>
       <c r="G2" s="21">
         <f>0.5*INT(F2/0.5)+INT( ((F2-INT(F2/0.5)*0.5)/0.25))*0.5</f>
@@ -4796,7 +4920,7 @@
       </c>
       <c r="B3" s="21">
         <f>Quiz!V3</f>
-        <v>0.75555555555555554</v>
+        <v>0.65833333333333333</v>
       </c>
       <c r="C3" s="20">
         <f>Homework!L3</f>
@@ -4812,11 +4936,11 @@
       </c>
       <c r="F3" s="21">
         <f t="shared" si="0"/>
-        <v>0.75555555555555554</v>
+        <v>0.65833333333333333</v>
       </c>
       <c r="G3" s="21">
         <f t="shared" ref="G3:G19" si="1">0.5*INT(F3/0.5)+INT( ((F3-INT(F3/0.5)*0.5)/0.25))*0.5</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="19">
         <f t="shared" ref="H3:H19" si="2">IF(G3&gt;4.75,1,0)</f>
@@ -4862,7 +4986,7 @@
       </c>
       <c r="B5" s="21">
         <f>Quiz!V5</f>
-        <v>0.53333333333333333</v>
+        <v>0.45</v>
       </c>
       <c r="C5" s="20">
         <f>Homework!L5</f>
@@ -4878,7 +5002,7 @@
       </c>
       <c r="F5" s="21">
         <f t="shared" si="0"/>
-        <v>0.53333333333333333</v>
+        <v>0.45</v>
       </c>
       <c r="G5" s="21">
         <f t="shared" si="1"/>
@@ -4895,7 +5019,7 @@
       </c>
       <c r="B6" s="21">
         <f>Quiz!V6</f>
-        <v>0.92222222222222228</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="C6" s="20">
         <f>Homework!L6</f>
@@ -4911,11 +5035,11 @@
       </c>
       <c r="F6" s="21">
         <f t="shared" si="0"/>
-        <v>0.92222222222222228</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="19">
         <f t="shared" si="2"/>
@@ -4928,7 +5052,7 @@
       </c>
       <c r="B7" s="21">
         <f>Quiz!V7</f>
-        <v>0.87777777777777777</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="C7" s="20">
         <f>Homework!L7</f>
@@ -4944,11 +5068,11 @@
       </c>
       <c r="F7" s="21">
         <f t="shared" si="0"/>
-        <v>0.87777777777777777</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="G7" s="21">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="19">
         <f t="shared" si="2"/>
@@ -4961,7 +5085,7 @@
       </c>
       <c r="B8" s="21">
         <f>Quiz!V8</f>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="C8" s="20">
         <f>Homework!L8</f>
@@ -4977,7 +5101,7 @@
       </c>
       <c r="F8" s="21">
         <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="G8" s="21">
         <f t="shared" si="1"/>
@@ -4994,7 +5118,7 @@
       </c>
       <c r="B9" s="21">
         <f>Quiz!V9</f>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
       <c r="C9" s="20">
         <f>Homework!L9</f>
@@ -5010,11 +5134,11 @@
       </c>
       <c r="F9" s="21">
         <f t="shared" si="0"/>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
       <c r="G9" s="21">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H9" s="19">
         <f t="shared" si="2"/>
@@ -5027,7 +5151,7 @@
       </c>
       <c r="B10" s="21">
         <f>Quiz!V10</f>
-        <v>0.73333333333333328</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="C10" s="20">
         <f>Homework!L10</f>
@@ -5043,7 +5167,7 @@
       </c>
       <c r="F10" s="21">
         <f t="shared" si="0"/>
-        <v>0.73333333333333328</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="G10" s="21">
         <f t="shared" si="1"/>
@@ -5093,7 +5217,7 @@
       </c>
       <c r="B12" s="21">
         <f>Quiz!V12</f>
-        <v>6.6666666666666666E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C12" s="20">
         <f>Homework!L12</f>
@@ -5109,7 +5233,7 @@
       </c>
       <c r="F12" s="21">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G12" s="21">
         <f t="shared" si="1"/>
@@ -5126,7 +5250,7 @@
       </c>
       <c r="B13" s="21">
         <f>Quiz!V13</f>
-        <v>0.36666666666666664</v>
+        <v>0.3</v>
       </c>
       <c r="C13" s="20">
         <f>Homework!L13</f>
@@ -5142,7 +5266,7 @@
       </c>
       <c r="F13" s="21">
         <f t="shared" si="0"/>
-        <v>0.36666666666666664</v>
+        <v>0.3</v>
       </c>
       <c r="G13" s="21">
         <f t="shared" si="1"/>
@@ -5159,7 +5283,7 @@
       </c>
       <c r="B14" s="21">
         <f>Quiz!V14</f>
-        <v>0.56666666666666665</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="C14" s="20">
         <f>Homework!L14</f>
@@ -5175,7 +5299,7 @@
       </c>
       <c r="F14" s="21">
         <f t="shared" si="0"/>
-        <v>0.56666666666666665</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="G14" s="21">
         <f t="shared" si="1"/>
@@ -5192,7 +5316,7 @@
       </c>
       <c r="B15" s="21">
         <f>Quiz!V15</f>
-        <v>1</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="C15" s="20">
         <f>Homework!L15</f>
@@ -5208,7 +5332,7 @@
       </c>
       <c r="F15" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="G15" s="21">
         <f t="shared" si="1"/>
@@ -5225,7 +5349,7 @@
       </c>
       <c r="B16" s="21">
         <f>Quiz!V16</f>
-        <v>0.73333333333333328</v>
+        <v>0.6</v>
       </c>
       <c r="C16" s="20">
         <f>Homework!L16</f>
@@ -5241,7 +5365,7 @@
       </c>
       <c r="F16" s="21">
         <f t="shared" si="0"/>
-        <v>0.73333333333333328</v>
+        <v>0.6</v>
       </c>
       <c r="G16" s="21">
         <f t="shared" si="1"/>
@@ -5258,7 +5382,7 @@
       </c>
       <c r="B17" s="21">
         <f>Quiz!V17</f>
-        <v>0.72222222222222221</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C17" s="20">
         <f>Homework!L17</f>
@@ -5274,7 +5398,7 @@
       </c>
       <c r="F17" s="21">
         <f t="shared" si="0"/>
-        <v>0.72222222222222221</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G17" s="21">
         <f t="shared" si="1"/>
@@ -5291,7 +5415,7 @@
       </c>
       <c r="B18" s="21">
         <f>Quiz!V18</f>
-        <v>0.7</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="C18" s="20">
         <f>Homework!L18</f>
@@ -5307,7 +5431,7 @@
       </c>
       <c r="F18" s="21">
         <f>$B18+$C18+($D18/100)*3+($E18/$E$35)*4.5</f>
-        <v>0.7</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="G18" s="21">
         <f t="shared" si="1"/>
@@ -5324,7 +5448,7 @@
       </c>
       <c r="B19" s="21">
         <f>Quiz!V19</f>
-        <v>0.66666666666666663</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C19" s="20">
         <f>Homework!L19</f>
@@ -5340,7 +5464,7 @@
       </c>
       <c r="F19" s="21">
         <f t="shared" ref="F19:F33" si="3">$B19+$C19+($D19/$D$35)*3+($E19/$E$35)*4.5</f>
-        <v>0.66666666666666663</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G19" s="21">
         <f t="shared" si="1"/>
@@ -5357,7 +5481,7 @@
       </c>
       <c r="B20" s="21">
         <f>Quiz!V20</f>
-        <v>0.43333333333333335</v>
+        <v>0.35</v>
       </c>
       <c r="C20" s="20">
         <f>Homework!L20</f>
@@ -5373,7 +5497,7 @@
       </c>
       <c r="F20" s="21">
         <f t="shared" si="3"/>
-        <v>0.43333333333333335</v>
+        <v>0.35</v>
       </c>
       <c r="G20" s="21">
         <f t="shared" ref="G20:G25" si="4">0.5*INT(F20/0.5)+INT( ((F20-INT(F20/0.5)*0.5)/0.25))*0.5</f>
@@ -5390,7 +5514,7 @@
       </c>
       <c r="B21" s="21">
         <f>Quiz!V21</f>
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="C21" s="20">
         <f>Homework!L21</f>
@@ -5406,11 +5530,11 @@
       </c>
       <c r="F21" s="21">
         <f t="shared" si="3"/>
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="G21" s="21">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H21" s="19">
         <f t="shared" si="5"/>
@@ -5423,7 +5547,7 @@
       </c>
       <c r="B22" s="21">
         <f>Quiz!V22</f>
-        <v>0.75555555555555554</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="C22" s="20">
         <f>Homework!L22</f>
@@ -5439,11 +5563,11 @@
       </c>
       <c r="F22" s="21">
         <f t="shared" si="3"/>
-        <v>0.75555555555555554</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="G22" s="21">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H22" s="19">
         <f t="shared" si="5"/>
@@ -5456,7 +5580,7 @@
       </c>
       <c r="B23" s="21">
         <f>Quiz!V23</f>
-        <v>0.53333333333333333</v>
+        <v>0.45</v>
       </c>
       <c r="C23" s="20">
         <f>Homework!L23</f>
@@ -5472,7 +5596,7 @@
       </c>
       <c r="F23" s="21">
         <f t="shared" si="3"/>
-        <v>0.53333333333333333</v>
+        <v>0.45</v>
       </c>
       <c r="G23" s="21">
         <f t="shared" si="4"/>
@@ -5489,7 +5613,7 @@
       </c>
       <c r="B24" s="21">
         <f>Quiz!V24</f>
-        <v>0.53333333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="C24" s="20">
         <f>Homework!L24</f>
@@ -5505,7 +5629,7 @@
       </c>
       <c r="F24" s="21">
         <f t="shared" si="3"/>
-        <v>0.53333333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="G24" s="21">
         <f t="shared" si="4"/>
@@ -5522,7 +5646,7 @@
       </c>
       <c r="B25" s="21">
         <f>Quiz!V25</f>
-        <v>0.5</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="C25" s="20">
         <f>Homework!L25</f>
@@ -5538,7 +5662,7 @@
       </c>
       <c r="F25" s="21">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="G25" s="21">
         <f t="shared" si="4"/>
@@ -5555,7 +5679,7 @@
       </c>
       <c r="B26" s="21">
         <f>Quiz!V26</f>
-        <v>0.53333333333333333</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C26" s="20">
         <f>Homework!L26</f>
@@ -5571,7 +5695,7 @@
       </c>
       <c r="F26" s="21">
         <f t="shared" si="3"/>
-        <v>0.53333333333333333</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G26" s="21">
         <f t="shared" ref="G26:G33" si="6">0.5*INT(F26/0.5)+INT( ((F26-INT(F26/0.5)*0.5)/0.25))*0.5</f>
@@ -5588,7 +5712,7 @@
       </c>
       <c r="B27" s="21">
         <f>Quiz!V27</f>
-        <v>0.65555555555555556</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="C27" s="20">
         <f>Homework!L27</f>
@@ -5604,7 +5728,7 @@
       </c>
       <c r="F27" s="21">
         <f t="shared" si="3"/>
-        <v>0.65555555555555556</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="G27" s="21">
         <f t="shared" si="6"/>
@@ -5621,7 +5745,7 @@
       </c>
       <c r="B28" s="21">
         <f>Quiz!V28</f>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="C28" s="20">
         <f>Homework!L28</f>
@@ -5637,7 +5761,7 @@
       </c>
       <c r="F28" s="21">
         <f t="shared" si="3"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="G28" s="21">
         <f t="shared" si="6"/>
@@ -5654,7 +5778,7 @@
       </c>
       <c r="B29" s="21">
         <f>Quiz!V29</f>
-        <v>0.7</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C29" s="20">
         <f>Homework!L29</f>
@@ -5670,7 +5794,7 @@
       </c>
       <c r="F29" s="21">
         <f t="shared" si="3"/>
-        <v>0.7</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G29" s="21">
         <f t="shared" si="6"/>
@@ -5687,7 +5811,7 @@
       </c>
       <c r="B30" s="21">
         <f>Quiz!V30</f>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="C30" s="20">
         <f>Homework!L30</f>
@@ -5703,7 +5827,7 @@
       </c>
       <c r="F30" s="21">
         <f t="shared" si="3"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="G30" s="21">
         <f t="shared" si="6"/>
@@ -5720,7 +5844,7 @@
       </c>
       <c r="B31" s="21">
         <f>Quiz!V31</f>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="C31" s="20">
         <f>Homework!L31</f>
@@ -5736,7 +5860,7 @@
       </c>
       <c r="F31" s="21">
         <f t="shared" si="3"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="G31" s="21">
         <f t="shared" si="6"/>
@@ -5753,7 +5877,7 @@
       </c>
       <c r="B32" s="21">
         <f>Quiz!V32</f>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="C32" s="20">
         <f>Homework!L32</f>
@@ -5769,7 +5893,7 @@
       </c>
       <c r="F32" s="21">
         <f t="shared" si="3"/>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="G32" s="21">
         <f t="shared" si="6"/>
@@ -5786,7 +5910,7 @@
       </c>
       <c r="B33" s="21">
         <f>Quiz!V33</f>
-        <v>0.75555555555555554</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="C33" s="20">
         <f>Homework!L33</f>
@@ -5802,11 +5926,11 @@
       </c>
       <c r="F33" s="21">
         <f t="shared" si="3"/>
-        <v>0.75555555555555554</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="G33" s="21">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H33" s="19">
         <f t="shared" si="7"/>
@@ -5859,7 +5983,7 @@
       </c>
       <c r="B36" s="35">
         <f t="shared" ref="B36:H36" si="8">AVERAGE(B$2:B$33)</f>
-        <v>0.5586805555555554</v>
+        <v>0.46484375000000011</v>
       </c>
       <c r="C36" s="35">
         <f t="shared" si="8"/>
@@ -5875,11 +5999,11 @@
       </c>
       <c r="F36" s="35">
         <f t="shared" si="8"/>
-        <v>0.5586805555555554</v>
+        <v>0.46484375000000011</v>
       </c>
       <c r="G36" s="35">
         <f t="shared" si="8"/>
-        <v>0.5625</v>
+        <v>0.453125</v>
       </c>
       <c r="H36" s="35">
         <f t="shared" si="8"/>
@@ -5892,7 +6016,7 @@
       </c>
       <c r="B37" s="35">
         <f t="shared" ref="B37:H37" si="9">STDEV(B$2:B$33)</f>
-        <v>0.24232108690680965</v>
+        <v>0.19930136012094168</v>
       </c>
       <c r="C37" s="35">
         <f t="shared" si="9"/>
@@ -5908,11 +6032,11 @@
       </c>
       <c r="F37" s="35">
         <f t="shared" si="9"/>
-        <v>0.24232108690680965</v>
+        <v>0.19930136012094168</v>
       </c>
       <c r="G37" s="35">
         <f t="shared" si="9"/>
-        <v>0.27679035970533089</v>
+        <v>0.1950754609987401</v>
       </c>
       <c r="H37" s="35">
         <f t="shared" si="9"/>
@@ -5925,7 +6049,7 @@
       </c>
       <c r="B38" s="35">
         <f t="shared" ref="B38:H38" si="10">MEDIAN(B$2:B$33)</f>
-        <v>0.53333333333333333</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="C38" s="35">
         <f t="shared" si="10"/>
@@ -5941,7 +6065,7 @@
       </c>
       <c r="F38" s="35">
         <f t="shared" si="10"/>
-        <v>0.53333333333333333</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="G38" s="35">
         <f t="shared" si="10"/>

</xml_diff>